<commit_message>
Made SpaceTypes strongly typed.
</commit_message>
<xml_diff>
--- a/Monopoly/Monopoly.Tests/TestData/BoardSpaces.xlsx
+++ b/Monopoly/Monopoly.Tests/TestData/BoardSpaces.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roger\source\repos\creyke\Monopoly\Monopoly\Monopoly.Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roger\source\repos\creyke\Monopoly\Monopoly\Monopoly.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56A6C8A-8DFA-4D23-8BC8-89B280A24BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9485D9D-FEA6-421D-9112-19C50F4A4C60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{21BCDE46-36CE-41B6-AD31-30F43975F69C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Bishopsgate</t>
   </si>
@@ -153,9 +153,6 @@
     <t>CostPerApt</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Super Tax</t>
   </si>
   <si>
-    <t>IncomeTax</t>
-  </si>
-  <si>
     <t>Jail</t>
   </si>
   <si>
@@ -229,6 +223,9 @@
   </si>
   <si>
     <t>PropertyGroup</t>
+  </si>
+  <si>
+    <t>SpaceType</t>
   </si>
 </sst>
 </file>
@@ -595,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C849C-E2EC-4782-9ACE-51E784D1A8EE}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -614,16 +611,16 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>32</v>
@@ -658,10 +655,10 @@
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="5"/>
       <c r="F2" s="5"/>
@@ -679,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -724,10 +721,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -785,10 +782,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
       <c r="D6" s="4">
         <v>1000000</v>
@@ -796,10 +793,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
       <c r="F7" s="4">
         <v>2000000</v>
@@ -860,10 +857,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -970,10 +967,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1027,10 +1024,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F14" s="4">
         <v>1500000</v>
@@ -1144,10 +1141,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="4">
         <v>2000000</v>
@@ -1207,10 +1204,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1317,10 +1314,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1373,10 +1370,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1483,10 +1480,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="4">
         <v>2000000</v>
@@ -1599,10 +1596,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F30" s="4">
         <v>1500000</v>
@@ -1663,10 +1660,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1772,10 +1769,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1828,10 +1825,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F37" s="4">
         <v>2000000</v>
@@ -1843,10 +1840,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1898,10 +1895,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D40" s="4">
         <v>2000000</v>

</xml_diff>